<commit_message>
Started to deal with betas
</commit_message>
<xml_diff>
--- a/sheets/input/Blank_Input.xlsx
+++ b/sheets/input/Blank_Input.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="115">
   <si>
     <t>Number of Hyper-cube bins</t>
   </si>
@@ -383,9 +383,6 @@
   </si>
   <si>
     <t>Attraction Factor 1</t>
-  </si>
-  <si>
-    <t>Phytoplankon</t>
   </si>
 </sst>
 </file>
@@ -1292,16 +1289,16 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4883,100 +4880,100 @@
       </c>
     </row>
     <row r="35" spans="5:6">
-      <c r="E35" s="81" t="s">
+      <c r="E35" s="79" t="s">
         <v>93</v>
       </c>
-      <c r="F35" s="81" t="s">
+      <c r="F35" s="79" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="36" spans="5:6">
-      <c r="E36" s="82"/>
-      <c r="F36" s="82"/>
+      <c r="E36" s="80"/>
+      <c r="F36" s="80"/>
     </row>
     <row r="37" spans="5:6">
-      <c r="E37" s="79" t="s">
+      <c r="E37" s="81" t="s">
         <v>95</v>
       </c>
-      <c r="F37" s="79" t="s">
+      <c r="F37" s="81" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="38" spans="5:6">
-      <c r="E38" s="80"/>
-      <c r="F38" s="80"/>
+      <c r="E38" s="82"/>
+      <c r="F38" s="82"/>
     </row>
     <row r="39" spans="5:6">
-      <c r="E39" s="79" t="s">
+      <c r="E39" s="81" t="s">
         <v>97</v>
       </c>
-      <c r="F39" s="79" t="s">
+      <c r="F39" s="81" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="40" spans="5:6">
-      <c r="E40" s="80"/>
-      <c r="F40" s="80"/>
+      <c r="E40" s="82"/>
+      <c r="F40" s="82"/>
     </row>
     <row r="41" spans="5:6">
-      <c r="E41" s="79" t="s">
+      <c r="E41" s="81" t="s">
         <v>99</v>
       </c>
-      <c r="F41" s="79" t="s">
+      <c r="F41" s="81" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="42" spans="5:6">
-      <c r="E42" s="80"/>
-      <c r="F42" s="80"/>
+      <c r="E42" s="82"/>
+      <c r="F42" s="82"/>
     </row>
     <row r="43" spans="5:6">
-      <c r="E43" s="79" t="s">
+      <c r="E43" s="81" t="s">
         <v>101</v>
       </c>
-      <c r="F43" s="79" t="s">
+      <c r="F43" s="81" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="44" spans="5:6">
-      <c r="E44" s="80"/>
-      <c r="F44" s="80"/>
+      <c r="E44" s="82"/>
+      <c r="F44" s="82"/>
     </row>
     <row r="45" spans="5:6">
-      <c r="E45" s="79" t="s">
+      <c r="E45" s="81" t="s">
         <v>103</v>
       </c>
-      <c r="F45" s="79" t="s">
+      <c r="F45" s="81" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="46" spans="5:6">
-      <c r="E46" s="80"/>
-      <c r="F46" s="80"/>
+      <c r="E46" s="82"/>
+      <c r="F46" s="82"/>
     </row>
     <row r="47" spans="5:6">
-      <c r="E47" s="79" t="s">
+      <c r="E47" s="81" t="s">
         <v>104</v>
       </c>
-      <c r="F47" s="79" t="s">
+      <c r="F47" s="81" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="48" spans="5:6">
-      <c r="E48" s="80"/>
-      <c r="F48" s="80"/>
+      <c r="E48" s="82"/>
+      <c r="F48" s="82"/>
     </row>
     <row r="49" spans="5:6">
-      <c r="E49" s="79" t="s">
+      <c r="E49" s="81" t="s">
         <v>106</v>
       </c>
-      <c r="F49" s="79" t="s">
+      <c r="F49" s="81" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="50" spans="5:6">
-      <c r="E50" s="80"/>
-      <c r="F50" s="80"/>
+      <c r="E50" s="82"/>
+      <c r="F50" s="82"/>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="74" t="s">
@@ -4990,12 +4987,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
     <mergeCell ref="E47:E48"/>
     <mergeCell ref="F47:F48"/>
     <mergeCell ref="E49:E50"/>
@@ -5006,6 +4997,12 @@
     <mergeCell ref="F43:F44"/>
     <mergeCell ref="E45:E46"/>
     <mergeCell ref="F45:F46"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5565,7 +5562,7 @@
         <v>10</v>
       </c>
       <c r="K2" s="25" t="s">
-        <v>115</v>
+        <v>21</v>
       </c>
       <c r="L2" s="25"/>
     </row>

</xml_diff>